<commit_message>
Reworked the global frequency table to increase efficiency. Made corresponding XLSX sheet to update the table.
</commit_message>
<xml_diff>
--- a/Global APRS Frequency.xlsx
+++ b/Global APRS Frequency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15da9958d5653d7c/Git/ptSolar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{F6EE69BA-721B-4835-B9B2-A7584B0BC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1AB966-FFEE-4492-98FF-3E5C5C50DA0F}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{F6EE69BA-721B-4835-B9B2-A7584B0BC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0240414-2CAF-4A20-A402-59AEA4893A22}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="3195" windowWidth="23040" windowHeight="12105" activeTab="1" xr2:uid="{AAA536C9-EB9E-420E-A518-398E663B386B}"/>
+    <workbookView xWindow="-30840" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{AAA536C9-EB9E-420E-A518-398E663B386B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Country/Area</t>
   </si>
@@ -61,6 +61,141 @@
   </si>
   <si>
     <t>000.0000</t>
+  </si>
+  <si>
+    <t>144.3900</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Transmit Prohibit</t>
+  </si>
+  <si>
+    <t>US and most of SA</t>
+  </si>
+  <si>
+    <t>145.5700</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>144.6600</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>145.5300</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>144.5250</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>144.6400</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>144.5750</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>145.1750</t>
+  </si>
+  <si>
+    <t>Austrailia</t>
+  </si>
+  <si>
+    <t>144.8000</t>
+  </si>
+  <si>
+    <t>EU and Africa</t>
+  </si>
+  <si>
+    <t>ISS and other Sats</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>TL Lat DDMM</t>
+  </si>
+  <si>
+    <t>TL Lon DDDMM</t>
+  </si>
+  <si>
+    <t>BR Lat DDMM</t>
+  </si>
+  <si>
+    <t>BR Lon DDDMM</t>
+  </si>
+  <si>
+    <t>TL Lat Int</t>
+  </si>
+  <si>
+    <t>TL Lon Int</t>
+  </si>
+  <si>
+    <t>BR Lat Int</t>
+  </si>
+  <si>
+    <t>BR Lon Int</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>US Canada Mexico</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Indonesia/Malaysia/Singapore</t>
+  </si>
+  <si>
+    <t>China/Taiwan</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>145.8250</t>
+  </si>
+  <si>
+    <t>// Transmit geo-lookups from east specific, to most specific. Transmit prohibits must be at the bottom of this list.</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;kml xmlns="http://www.opengis.net/kml/2.2"&gt;&lt;Document&gt;&lt;name&gt;APRS Frequency Worldwide&lt;/name&gt;&lt;description/&gt;&lt;Style id="poly-000000-1200-77-nodesc-normal"&gt;&lt;LineStyle&gt;&lt;color&gt;ff000000&lt;/color&gt;&lt;width&gt;1.2&lt;/width&gt;&lt;/LineStyle&gt;&lt;PolyStyle&gt;&lt;color&gt;4d000000&lt;/color&gt;&lt;fill&gt;1&lt;/fill&gt;&lt;outline&gt;1&lt;/outline&gt;&lt;/PolyStyle&gt;&lt;BalloonStyle&gt;&lt;text&gt;&lt;![CDATA[&lt;h3&gt;$[name]&lt;/h3&gt;]]&gt;&lt;/text&gt;&lt;/BalloonStyle&gt;&lt;/Style&gt;&lt;Style id="poly-000000-1200-77-nodesc-highlight"&gt;&lt;LineStyle&gt;&lt;color&gt;ff000000&lt;/color&gt;&lt;width&gt;1.8&lt;/width&gt;&lt;/LineStyle&gt;&lt;PolyStyle&gt;&lt;color&gt;4d000000&lt;/color&gt;&lt;fill&gt;1&lt;/fill&gt;&lt;outline&gt;1&lt;/outline&gt;&lt;/PolyStyle&gt;&lt;BalloonStyle&gt;&lt;text&gt;&lt;![CDATA[&lt;h3&gt;$[name]&lt;/h3&gt;]]&gt;&lt;/text&gt;&lt;/BalloonStyle&gt;&lt;/Style&gt;&lt;StyleMap id="poly-000000-1200-77-nodesc"&gt;&lt;Pair&gt;&lt;key&gt;normal&lt;/key&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc-normal&lt;/styleUrl&gt;&lt;/Pair&gt;&lt;Pair&gt;&lt;key&gt;highlight&lt;/key&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc-highlight&lt;/styleUrl&gt;&lt;/Pair&gt;&lt;/StyleMap&gt;&lt;Folder&gt;&lt;name&gt;Untitled layer&lt;/name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/Folder&gt;&lt;/Document&gt;&lt;/kml&gt;</t>
   </si>
 </sst>
 </file>
@@ -114,6 +249,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCDA1C44-C667-4DAD-8E73-520F3AF7EAD9}" name="Freq" displayName="Freq" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12" xr:uid="{FCDA1C44-C667-4DAD-8E73-520F3AF7EAD9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2FF38C14-C6FA-4B6D-8B08-3AC03AE936F9}" name="Freq #"/>
+    <tableColumn id="2" xr3:uid="{B14E7841-A258-4D86-8DFA-E081812C516E}" name="Frequency"/>
+    <tableColumn id="3" xr3:uid="{9B1A4D36-8CC3-4A88-9BF3-2A27E1C7BDD5}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,15 +584,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E0E84B-60E6-4C01-8777-8C0ABA3794D9}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="114.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,44 +623,1354 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>-130</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>-34</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>VLOOKUP(F2, Freq[], 2, TRUE)</f>
+        <v>144.3900</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H8" si="0">TEXT(INT(B2),"00") &amp; TEXT((B2-INT(B2))*60,"00")</f>
+        <v>8000</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I8" si="1">TEXT(INT(C2),"000") &amp; TEXT((C2-INT(C2))*60,"00")</f>
+        <v>-13000</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J8" si="2">TEXT(INT(D2),"00") &amp; TEXT((D2-INT(D2))*60,"00")</f>
+        <v>0000</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K8" si="3">TEXT(INT(E2),"000") &amp; TEXT((E2-INT(E2))*60,"00")</f>
+        <v>-03400</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L8" si="4">INT(H2)</f>
+        <v>8000</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M8" si="5">INT(I2)</f>
+        <v>-13000</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N8" si="6">INT(J2)</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O8" si="7">INT(K2)</f>
+        <v>-3400</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>_xlfn.CONCAT("if (iLat &gt;= ", N2, " &amp;&amp; iLat &lt;= ", L2, " &amp;&amp; iLon &gt;= ", M2, " &amp;&amp; iLon &lt;= ", O2, ") freqSelected = ", F2, ";    //", A2, " on ", G2, "MHz")</f>
+        <v>if (iLat &gt;= 0 &amp;&amp; iLat &lt;= 8000 &amp;&amp; iLon &gt;= -13000 &amp;&amp; iLon &lt;= -3400) freqSelected = 1;    //US Canada Mexico on 144.3900MHz</v>
+      </c>
+      <c r="S2" t="str">
+        <f>_xlfn.CONCAT("&lt;Placemark&gt;&lt;name&gt;",A2, " on ", G2, "MHz","&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;",C2, ",", B2, ",0 ",E2, ",", B2, ",0 ",E2, ",", D2, ",0 ",C2, ",", D2, ",0 ",C2, ",", B2, ",0 ","&lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;")</f>
+        <v>&lt;Placemark&gt;&lt;name&gt;US Canada Mexico on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-130,80,0 -34,80,0 -34,0,0 -130,0,0 -130,80,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-103</v>
+      </c>
+      <c r="D3">
+        <v>-60</v>
+      </c>
+      <c r="E3">
+        <v>-33</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>VLOOKUP(F3, Freq[], 2, TRUE)</f>
+        <v>144.3900</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="1"/>
+        <v>-10300</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="2"/>
+        <v>-6000</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="3"/>
+        <v>-03300</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="5"/>
+        <v>-10300</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="6"/>
+        <v>-6000</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="7"/>
+        <v>-3300</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q19" si="8">_xlfn.CONCAT("if (iLat &gt;= ", N3, " &amp;&amp; iLat &lt;= ", L3, " &amp;&amp; iLon &gt;= ", M3, " &amp;&amp; iLon &lt;= ", O3, ") freqSelected = ", F3, ";    //", A3, " on ", G3, "MHz")</f>
+        <v>if (iLat &gt;= -6000 &amp;&amp; iLat &lt;= 0 &amp;&amp; iLon &gt;= -10300 &amp;&amp; iLon &lt;= -3300) freqSelected = 1;    //South America on 144.3900MHz</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S19" si="9">_xlfn.CONCAT("&lt;Placemark&gt;&lt;name&gt;",A3, " on ", G3, "MHz","&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;",C3, ",", B3, ",0 ",E3, ",", B3, ",0 ",E3, ",", D3, ",0 ",C3, ",", D3, ",0 ",C3, ",", B3, ",0 ","&lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;")</f>
+        <v>&lt;Placemark&gt;&lt;name&gt;South America on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-103,0,0 -33,0,0 -33,-60,0 -103,-60,0 -103,0,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>96</v>
+      </c>
+      <c r="D4">
+        <v>-10</v>
+      </c>
+      <c r="E4">
+        <v>142</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(F4, Freq[], 2, TRUE)</f>
+        <v>144.3900</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>09600</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="3"/>
+        <v>14200</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>9600</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="6"/>
+        <v>-1000</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="7"/>
+        <v>14200</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= -1000 &amp;&amp; iLat &lt;= 2000 &amp;&amp; iLon &gt;= 9600 &amp;&amp; iLon &lt;= 14200) freqSelected = 1;    //Indonesia/Malaysia/Singapore on 144.3900MHz</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Indonesia/Malaysia/Singapore on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;96,20,0 142,20,0 142,-10,0 96,-10,0 96,20,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>135</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(F5, Freq[], 2, TRUE)</f>
+        <v>144.6400</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>5200</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>06900</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v>13500</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>5200</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>6900</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="7"/>
+        <v>13500</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 2000 &amp;&amp; iLat &lt;= 5200 &amp;&amp; iLon &gt;= 6900 &amp;&amp; iLon &lt;= 13500) freqSelected = 4;    //China/Taiwan on 144.6400MHz</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;China/Taiwan on 144.6400MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;69,52,0 135,52,0 135,20,0 69,20,0 69,52,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>-32</v>
+      </c>
+      <c r="C6">
+        <v>165</v>
+      </c>
+      <c r="D6">
+        <v>-49</v>
+      </c>
+      <c r="E6">
+        <v>180</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(F6, Freq[], 2, TRUE)</f>
+        <v>144.5750</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>-3200</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>16500</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>-4900</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v>18000</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>-3200</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>16500</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="6"/>
+        <v>-4900</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="7"/>
+        <v>18000</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= -4900 &amp;&amp; iLat &lt;= -3200 &amp;&amp; iLon &gt;= 16500 &amp;&amp; iLon &lt;= 18000) freqSelected = 3;    //New Zealand on 144.5750MHz</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;New Zealand on 144.5750MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;165,-32,0 180,-32,0 180,-49,0 165,-49,0 165,-32,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>-9</v>
+      </c>
+      <c r="C7">
+        <v>111</v>
+      </c>
+      <c r="D7">
+        <v>-45</v>
+      </c>
+      <c r="E7">
+        <v>154</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(F7, Freq[], 2, TRUE)</f>
+        <v>145.1750</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>-0900</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>11100</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>-4500</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>15400</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>-900</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>11100</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="6"/>
+        <v>-4500</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="7"/>
+        <v>15400</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= -4500 &amp;&amp; iLat &lt;= -900 &amp;&amp; iLon &gt;= 11100 &amp;&amp; iLon &lt;= 15400) freqSelected = 7;    //Austrailia on 145.1750MHz</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Austrailia on 145.1750MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;111,-9,0 154,-9,0 154,-45,0 111,-45,0 111,-9,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>73</v>
+      </c>
+      <c r="C8">
+        <v>-12</v>
+      </c>
+      <c r="D8">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(F8, Freq[], 2, TRUE)</f>
+        <v>144.8000</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>7300</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>-01200</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>3600</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>05000</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>7300</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>-1200</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="6"/>
+        <v>3600</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="7"/>
+        <v>5000</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 3600 &amp;&amp; iLat &lt;= 7300 &amp;&amp; iLon &gt;= -1200 &amp;&amp; iLon &lt;= 5000) freqSelected = 6;    //Europe on 144.8000MHz</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Europe on 144.8000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-12,73,0 50,73,0 50,36,0 -12,36,0 -12,73,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>-21</v>
+      </c>
+      <c r="D9">
+        <v>-36</v>
+      </c>
+      <c r="E9">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(F9, Freq[], 2, TRUE)</f>
+        <v>144.8000</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" ref="H9:H10" si="10">TEXT(INT(B9),"00") &amp; TEXT((B9-INT(B9))*60,"00")</f>
+        <v>3600</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" ref="I9:I10" si="11">TEXT(INT(C9),"000") &amp; TEXT((C9-INT(C9))*60,"00")</f>
+        <v>-02100</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ref="J9:J10" si="12">TEXT(INT(D9),"00") &amp; TEXT((D9-INT(D9))*60,"00")</f>
+        <v>-3600</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" ref="K9:K10" si="13">TEXT(INT(E9),"000") &amp; TEXT((E9-INT(E9))*60,"00")</f>
+        <v>05200</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L10" si="14">INT(H9)</f>
+        <v>3600</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M10" si="15">INT(I9)</f>
+        <v>-2100</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:N10" si="16">INT(J9)</f>
+        <v>-3600</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O10" si="17">INT(K9)</f>
+        <v>5200</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= -3600 &amp;&amp; iLat &lt;= 3600 &amp;&amp; iLon &gt;= -2100 &amp;&amp; iLon &lt;= 5200) freqSelected = 6;    //Africa on 144.8000MHz</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Africa on 144.8000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-21,36,0 52,36,0 52,-36,0 -21,-36,0 -21,36,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>52</v>
+      </c>
+      <c r="E10">
+        <v>180</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(F10, Freq[], 2, TRUE)</f>
+        <v>144.8000</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="10"/>
+        <v>7500</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="11"/>
+        <v>05000</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="12"/>
+        <v>5200</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="13"/>
+        <v>18000</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="14"/>
+        <v>7500</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="15"/>
+        <v>5000</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="16"/>
+        <v>5200</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="17"/>
+        <v>18000</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 5200 &amp;&amp; iLat &lt;= 7500 &amp;&amp; iLon &gt;= 5000 &amp;&amp; iLon &lt;= 18000) freqSelected = 6;    //Russia on 144.8000MHz</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Russia on 144.8000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;50,75,0 180,75,0 180,52,0 50,52,0 50,75,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>-169</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>-130</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP(F11, Freq[], 2, TRUE)</f>
+        <v>144.3900</v>
+      </c>
+      <c r="H11" t="str">
+        <f>TEXT(INT(B11),"00") &amp; TEXT((B11-INT(B11))*60,"00")</f>
+        <v>8000</v>
+      </c>
+      <c r="I11" t="str">
+        <f>TEXT(INT(C11),"000") &amp; TEXT((C11-INT(C11))*60,"00")</f>
+        <v>-16900</v>
+      </c>
+      <c r="J11" t="str">
+        <f>TEXT(INT(D11),"00") &amp; TEXT((D11-INT(D11))*60,"00")</f>
+        <v>5000</v>
+      </c>
+      <c r="K11" t="str">
+        <f>TEXT(INT(E11),"000") &amp; TEXT((E11-INT(E11))*60,"00")</f>
+        <v>-13000</v>
+      </c>
+      <c r="L11">
+        <f>INT(H11)</f>
+        <v>8000</v>
+      </c>
+      <c r="M11">
+        <f>INT(I11)</f>
+        <v>-16900</v>
+      </c>
+      <c r="N11">
+        <f>INT(J11)</f>
+        <v>5000</v>
+      </c>
+      <c r="O11">
+        <f>INT(K11)</f>
+        <v>-13000</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 5000 &amp;&amp; iLat &lt;= 8000 &amp;&amp; iLon &gt;= -16900 &amp;&amp; iLon &lt;= -13000) freqSelected = 1;    //Alaska on 144.3900MHz</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Alaska on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-169,80,0 -130,80,0 -130,50,0 -169,50,0 -169,80,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>-165</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>-153</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(F12, Freq[], 2, TRUE)</f>
+        <v>144.3900</v>
+      </c>
+      <c r="H12" t="str">
+        <f>TEXT(INT(B12),"00") &amp; TEXT((B12-INT(B12))*60,"00")</f>
+        <v>2600</v>
+      </c>
+      <c r="I12" t="str">
+        <f>TEXT(INT(C12),"000") &amp; TEXT((C12-INT(C12))*60,"00")</f>
+        <v>-16500</v>
+      </c>
+      <c r="J12" t="str">
+        <f>TEXT(INT(D12),"00") &amp; TEXT((D12-INT(D12))*60,"00")</f>
+        <v>1500</v>
+      </c>
+      <c r="K12" t="str">
+        <f>TEXT(INT(E12),"000") &amp; TEXT((E12-INT(E12))*60,"00")</f>
+        <v>-15300</v>
+      </c>
+      <c r="L12">
+        <f>INT(H12)</f>
+        <v>2600</v>
+      </c>
+      <c r="M12">
+        <f>INT(I12)</f>
+        <v>-16500</v>
+      </c>
+      <c r="N12">
+        <f>INT(J12)</f>
+        <v>1500</v>
+      </c>
+      <c r="O12">
+        <f>INT(K12)</f>
+        <v>-15300</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 1500 &amp;&amp; iLat &lt;= 2600 &amp;&amp; iLon &gt;= -16500 &amp;&amp; iLon &lt;= -15300) freqSelected = 1;    //Hawaii on 144.3900MHz</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Hawaii on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-165,26,0 -153,26,0 -153,15,0 -165,15,0 -165,26,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>-70</v>
+      </c>
+      <c r="D13">
+        <v>-30</v>
+      </c>
+      <c r="E13">
+        <v>-33</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(F13, Freq[], 2, TRUE)</f>
+        <v>145.5700</v>
+      </c>
+      <c r="H13" t="str">
+        <f>TEXT(INT(B13),"00") &amp; TEXT((B13-INT(B13))*60,"00")</f>
+        <v>0300</v>
+      </c>
+      <c r="I13" t="str">
+        <f>TEXT(INT(C13),"000") &amp; TEXT((C13-INT(C13))*60,"00")</f>
+        <v>-07000</v>
+      </c>
+      <c r="J13" t="str">
+        <f>TEXT(INT(D13),"00") &amp; TEXT((D13-INT(D13))*60,"00")</f>
+        <v>-3000</v>
+      </c>
+      <c r="K13" t="str">
+        <f>TEXT(INT(E13),"000") &amp; TEXT((E13-INT(E13))*60,"00")</f>
+        <v>-03300</v>
+      </c>
+      <c r="L13">
+        <f>INT(H13)</f>
+        <v>300</v>
+      </c>
+      <c r="M13">
+        <f>INT(I13)</f>
+        <v>-7000</v>
+      </c>
+      <c r="N13">
+        <f>INT(J13)</f>
+        <v>-3000</v>
+      </c>
+      <c r="O13">
+        <f>INT(K13)</f>
+        <v>-3300</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= -3000 &amp;&amp; iLat &lt;= 300 &amp;&amp; iLon &gt;= -7000 &amp;&amp; iLon &lt;= -3300) freqSelected = 9;    //Brazil on 145.5700MHz</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Brazil on 145.5700MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-70,3,0 -33,3,0 -33,-30,0 -70,-30,0 -70,3,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>129</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>146</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(F14, Freq[], 2, TRUE)</f>
+        <v>144.6600</v>
+      </c>
+      <c r="H14" t="str">
+        <f>TEXT(INT(B14),"00") &amp; TEXT((B14-INT(B14))*60,"00")</f>
+        <v>4500</v>
+      </c>
+      <c r="I14" t="str">
+        <f>TEXT(INT(C14),"000") &amp; TEXT((C14-INT(C14))*60,"00")</f>
+        <v>12900</v>
+      </c>
+      <c r="J14" t="str">
+        <f>TEXT(INT(D14),"00") &amp; TEXT((D14-INT(D14))*60,"00")</f>
+        <v>3000</v>
+      </c>
+      <c r="K14" t="str">
+        <f>TEXT(INT(E14),"000") &amp; TEXT((E14-INT(E14))*60,"00")</f>
+        <v>14600</v>
+      </c>
+      <c r="L14">
+        <f>INT(H14)</f>
+        <v>4500</v>
+      </c>
+      <c r="M14">
+        <f>INT(I14)</f>
+        <v>12900</v>
+      </c>
+      <c r="N14">
+        <f>INT(J14)</f>
+        <v>3000</v>
+      </c>
+      <c r="O14">
+        <f>INT(K14)</f>
+        <v>14600</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 3000 &amp;&amp; iLat &lt;= 4500 &amp;&amp; iLon &gt;= 12900 &amp;&amp; iLon &lt;= 14600) freqSelected = 5;    //Japan on 144.6600MHz</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Japan on 144.6600MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;129,45,0 146,45,0 146,30,0 129,30,0 129,45,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>20.6</v>
+      </c>
+      <c r="C15">
+        <v>97</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>106</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(F15, Freq[], 2, TRUE)</f>
+        <v>145.5300</v>
+      </c>
+      <c r="H15" t="str">
+        <f>TEXT(INT(B15),"00") &amp; TEXT((B15-INT(B15))*60,"00")</f>
+        <v>2036</v>
+      </c>
+      <c r="I15" t="str">
+        <f>TEXT(INT(C15),"000") &amp; TEXT((C15-INT(C15))*60,"00")</f>
+        <v>09700</v>
+      </c>
+      <c r="J15" t="str">
+        <f>TEXT(INT(D15),"00") &amp; TEXT((D15-INT(D15))*60,"00")</f>
+        <v>0500</v>
+      </c>
+      <c r="K15" t="str">
+        <f>TEXT(INT(E15),"000") &amp; TEXT((E15-INT(E15))*60,"00")</f>
+        <v>10600</v>
+      </c>
+      <c r="L15">
+        <f>INT(H15)</f>
+        <v>2036</v>
+      </c>
+      <c r="M15">
+        <f>INT(I15)</f>
+        <v>9700</v>
+      </c>
+      <c r="N15">
+        <f>INT(J15)</f>
+        <v>500</v>
+      </c>
+      <c r="O15">
+        <f>INT(K15)</f>
+        <v>10600</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 500 &amp;&amp; iLat &lt;= 2036 &amp;&amp; iLon &gt;= 9700 &amp;&amp; iLon &lt;= 10600) freqSelected = 8;    //Thailand on 145.5300MHz</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Thailand on 145.5300MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;97,20.6,0 106,20.6,0 106,5,0 97,5,0 97,20.6,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>22.5</v>
+      </c>
+      <c r="C16">
+        <v>113.8</v>
+      </c>
+      <c r="D16">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <v>114.5</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(F16, Freq[], 2, TRUE)</f>
+        <v>144.5250</v>
+      </c>
+      <c r="H16" t="str">
+        <f>TEXT(INT(B16),"00") &amp; TEXT((B16-INT(B16))*60,"00")</f>
+        <v>2230</v>
+      </c>
+      <c r="I16" t="str">
+        <f>TEXT(INT(C16),"000") &amp; TEXT((C16-INT(C16))*60,"00")</f>
+        <v>11348</v>
+      </c>
+      <c r="J16" t="str">
+        <f>TEXT(INT(D16),"00") &amp; TEXT((D16-INT(D16))*60,"00")</f>
+        <v>2200</v>
+      </c>
+      <c r="K16" t="str">
+        <f>TEXT(INT(E16),"000") &amp; TEXT((E16-INT(E16))*60,"00")</f>
+        <v>11430</v>
+      </c>
+      <c r="L16">
+        <f>INT(H16)</f>
+        <v>2230</v>
+      </c>
+      <c r="M16">
+        <f>INT(I16)</f>
+        <v>11348</v>
+      </c>
+      <c r="N16">
+        <f>INT(J16)</f>
+        <v>2200</v>
+      </c>
+      <c r="O16">
+        <f>INT(K16)</f>
+        <v>11430</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 2200 &amp;&amp; iLat &lt;= 2230 &amp;&amp; iLon &gt;= 11348 &amp;&amp; iLon &lt;= 11430) freqSelected = 2;    //Hong Kong on 144.5250MHz</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Hong Kong on 144.5250MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;113.8,22.5,0 114.5,22.5,0 114.5,22,0 113.8,22,0 113.8,22.5,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <v>-8</v>
+      </c>
+      <c r="D17">
+        <v>49</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(F17, Freq[], 2, TRUE)</f>
+        <v>000.0000</v>
+      </c>
+      <c r="H17" t="str">
+        <f>TEXT(INT(B17),"00") &amp; TEXT((B17-INT(B17))*60,"00")</f>
+        <v>6100</v>
+      </c>
+      <c r="I17" t="str">
+        <f>TEXT(INT(C17),"000") &amp; TEXT((C17-INT(C17))*60,"00")</f>
+        <v>-00800</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ref="I17:K17" si="18">TEXT(INT(D17),"00") &amp; TEXT((D17-INT(D17))*60,"00")</f>
+        <v>4900</v>
+      </c>
+      <c r="K17" t="str">
+        <f>TEXT(INT(E17),"000") &amp; TEXT((E17-INT(E17))*60,"00")</f>
+        <v>00200</v>
+      </c>
+      <c r="L17">
+        <f>INT(H17)</f>
+        <v>6100</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17:O17" si="19">INT(I17)</f>
+        <v>-800</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="19"/>
+        <v>4900</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="19"/>
+        <v>200</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 4900 &amp;&amp; iLat &lt;= 6100 &amp;&amp; iLon &gt;= -800 &amp;&amp; iLon &lt;= 200) freqSelected = 0;    //UK on 000.0000MHz</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;UK on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-8,61,0 2,61,0 2,49,0 -8,49,0 -8,61,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>19.2</v>
+      </c>
+      <c r="C18">
+        <v>42</v>
+      </c>
+      <c r="D18">
+        <v>11.8</v>
+      </c>
+      <c r="E18">
+        <v>54.7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(F18, Freq[], 2, TRUE)</f>
+        <v>000.0000</v>
+      </c>
+      <c r="H18" t="str">
+        <f>TEXT(INT(B18),"00") &amp; TEXT((B18-INT(B18))*60,"00")</f>
+        <v>1912</v>
+      </c>
+      <c r="I18" t="str">
+        <f>TEXT(INT(C18),"000") &amp; TEXT((C18-INT(C18))*60,"00")</f>
+        <v>04200</v>
+      </c>
+      <c r="J18" t="str">
+        <f>TEXT(INT(D18),"00") &amp; TEXT((D18-INT(D18))*60,"00")</f>
+        <v>1148</v>
+      </c>
+      <c r="K18" t="str">
+        <f>TEXT(INT(E18),"000") &amp; TEXT((E18-INT(E18))*60,"00")</f>
+        <v>05442</v>
+      </c>
+      <c r="L18">
+        <f>INT(H18)</f>
+        <v>1912</v>
+      </c>
+      <c r="M18">
+        <f>INT(I18)</f>
+        <v>4200</v>
+      </c>
+      <c r="N18">
+        <f>INT(J18)</f>
+        <v>1148</v>
+      </c>
+      <c r="O18">
+        <f>INT(K18)</f>
+        <v>5442</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 1148 &amp;&amp; iLat &lt;= 1912 &amp;&amp; iLon &gt;= 4200 &amp;&amp; iLon &lt;= 5442) freqSelected = 0;    //Yemen on 000.0000MHz</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Yemen on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;42,19.2,0 54.7,19.2,0 54.7,11.8,0 42,11.8,0 42,19.2,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>43.1</v>
+      </c>
+      <c r="C19">
+        <v>131</v>
+      </c>
+      <c r="D19">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E19">
+        <v>124</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(F19, Freq[], 2, TRUE)</f>
+        <v>000.0000</v>
+      </c>
+      <c r="H19" t="str">
+        <f>TEXT(INT(B19),"00") &amp; TEXT((B19-INT(B19))*60,"00")</f>
+        <v>4306</v>
+      </c>
+      <c r="I19" t="str">
+        <f>TEXT(INT(C19),"000") &amp; TEXT((C19-INT(C19))*60,"00")</f>
+        <v>13100</v>
+      </c>
+      <c r="J19" t="str">
+        <f>TEXT(INT(D19),"00") &amp; TEXT((D19-INT(D19))*60,"00")</f>
+        <v>3742</v>
+      </c>
+      <c r="K19" t="str">
+        <f>TEXT(INT(E19),"000") &amp; TEXT((E19-INT(E19))*60,"00")</f>
+        <v>12400</v>
+      </c>
+      <c r="L19">
+        <f>INT(H19)</f>
+        <v>4306</v>
+      </c>
+      <c r="M19">
+        <f>INT(I19)</f>
+        <v>13100</v>
+      </c>
+      <c r="N19">
+        <f>INT(J19)</f>
+        <v>3742</v>
+      </c>
+      <c r="O19">
+        <f>INT(K19)</f>
+        <v>12400</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="8"/>
+        <v>if (iLat &gt;= 3742 &amp;&amp; iLat &lt;= 4306 &amp;&amp; iLon &gt;= 13100 &amp;&amp; iLon &lt;= 12400) freqSelected = 0;    //North Korea on 000.0000MHz</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;North Korea on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;131,43.1,0 124,43.1,0 124,37.7,0 131,37.7,0 131,43.1,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S25" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025CF16C-04A7-4E32-9707-D2C98FCC0F06}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>99</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C11">
+    <sortCondition ref="B4:B11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 1.1.0. Fixed bug in the geo-lookups, eliminated extra debug codes, enhanced the PT0100 config format, tweaked the delay logic when flying over xmit-prohibit areas.
</commit_message>
<xml_diff>
--- a/Global APRS Frequency.xlsx
+++ b/Global APRS Frequency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15da9958d5653d7c/Git/ptSolar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{F6EE69BA-721B-4835-B9B2-A7584B0BC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0240414-2CAF-4A20-A402-59AEA4893A22}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{F6EE69BA-721B-4835-B9B2-A7584B0BC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E19DAC05-CE0D-4463-AE11-5E797D2313DC}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{AAA536C9-EB9E-420E-A518-398E663B386B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AAA536C9-EB9E-420E-A518-398E663B386B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Country/Area</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>&lt;/Folder&gt;&lt;/Document&gt;&lt;/kml&gt;</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>South Hutch</t>
+  </si>
+  <si>
+    <t>Burrton</t>
+  </si>
+  <si>
+    <t>US50</t>
   </si>
 </sst>
 </file>
@@ -584,24 +596,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E0E84B-60E6-4C01-8777-8C0ABA3794D9}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="114.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="114.5546875" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +666,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -678,35 +690,35 @@
         <v>144.3900</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H8" si="0">TEXT(INT(B2),"00") &amp; TEXT((B2-INT(B2))*60,"00")</f>
+        <f>IF(B2&gt;=0,"","-") &amp; TEXT(INT(ABS(B2)),"00") &amp; TEXT(INT((ABS(B2)-INT(ABS(B2)))*60),"00")</f>
         <v>8000</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I8" si="1">TEXT(INT(C2),"000") &amp; TEXT((C2-INT(C2))*60,"00")</f>
+        <f>IF(C2&gt;=0,"","-") &amp; TEXT(INT(ABS(C2)),"000") &amp; TEXT(INT((ABS(C2)-INT(ABS(C2)))*60),"00")</f>
         <v>-13000</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J8" si="2">TEXT(INT(D2),"00") &amp; TEXT((D2-INT(D2))*60,"00")</f>
+        <f>IF(D2&gt;=0,"","-") &amp; TEXT(INT(ABS(D2)),"00") &amp; TEXT(INT((ABS(D2)-INT(ABS(D2)))*60),"00")</f>
         <v>0000</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K8" si="3">TEXT(INT(E2),"000") &amp; TEXT((E2-INT(E2))*60,"00")</f>
+        <f>IF(E2&gt;=0,"","-") &amp; TEXT(INT(ABS(E2)),"000") &amp; TEXT(INT((ABS(E2)-INT(ABS(E2)))*60),"00")</f>
         <v>-03400</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:L8" si="4">INT(H2)</f>
+        <f t="shared" ref="L2:L8" si="0">INT(H2)</f>
         <v>8000</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M8" si="5">INT(I2)</f>
+        <f t="shared" ref="M2:M8" si="1">INT(I2)</f>
         <v>-13000</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N8" si="6">INT(J2)</f>
+        <f t="shared" ref="N2:N8" si="2">INT(J2)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O8" si="7">INT(K2)</f>
+        <f t="shared" ref="O2:O8" si="3">INT(K2)</f>
         <v>-3400</v>
       </c>
       <c r="Q2" t="str">
@@ -718,7 +730,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;US Canada Mexico on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-130,80,0 -34,80,0 -34,0,0 -130,0,0 -130,80,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -742,35 +754,35 @@
         <v>144.3900</v>
       </c>
       <c r="H3" t="str">
+        <f t="shared" ref="H3:H19" si="4">IF(B3&gt;=0,"","-") &amp; TEXT(INT(ABS(B3)),"00") &amp; TEXT(INT((ABS(B3)-INT(ABS(B3)))*60),"00")</f>
+        <v>0000</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I19" si="5">IF(C3&gt;=0,"","-") &amp; TEXT(INT(ABS(C3)),"000") &amp; TEXT(INT((ABS(C3)-INT(ABS(C3)))*60),"00")</f>
+        <v>-10300</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J19" si="6">IF(D3&gt;=0,"","-") &amp; TEXT(INT(ABS(D3)),"00") &amp; TEXT(INT((ABS(D3)-INT(ABS(D3)))*60),"00")</f>
+        <v>-6000</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K19" si="7">IF(E3&gt;=0,"","-") &amp; TEXT(INT(ABS(E3)),"000") &amp; TEXT(INT((ABS(E3)-INT(ABS(E3)))*60),"00")</f>
+        <v>-03300</v>
+      </c>
+      <c r="L3">
         <f t="shared" si="0"/>
-        <v>0000</v>
-      </c>
-      <c r="I3" t="str">
+        <v>0</v>
+      </c>
+      <c r="M3">
         <f t="shared" si="1"/>
         <v>-10300</v>
       </c>
-      <c r="J3" t="str">
+      <c r="N3">
         <f t="shared" si="2"/>
         <v>-6000</v>
       </c>
-      <c r="K3" t="str">
+      <c r="O3">
         <f t="shared" si="3"/>
-        <v>-03300</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="5"/>
-        <v>-10300</v>
-      </c>
-      <c r="N3">
-        <f t="shared" si="6"/>
-        <v>-6000</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="7"/>
         <v>-3300</v>
       </c>
       <c r="Q3" t="str">
@@ -782,7 +794,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;South America on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-103,0,0 -33,0,0 -33,-60,0 -103,-60,0 -103,0,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -806,35 +818,35 @@
         <v>144.3900</v>
       </c>
       <c r="H4" t="str">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="5"/>
+        <v>09600</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="6"/>
+        <v>-1000</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="7"/>
+        <v>14200</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="I4" t="str">
+      <c r="M4">
         <f t="shared" si="1"/>
-        <v>09600</v>
-      </c>
-      <c r="J4" t="str">
+        <v>9600</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="2"/>
         <v>-1000</v>
       </c>
-      <c r="K4" t="str">
+      <c r="O4">
         <f t="shared" si="3"/>
-        <v>14200</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="4"/>
-        <v>2000</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="5"/>
-        <v>9600</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="6"/>
-        <v>-1000</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="7"/>
         <v>14200</v>
       </c>
       <c r="Q4" t="str">
@@ -846,7 +858,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Indonesia/Malaysia/Singapore on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;96,20,0 142,20,0 142,-10,0 96,-10,0 96,20,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -870,35 +882,35 @@
         <v>144.6400</v>
       </c>
       <c r="H5" t="str">
+        <f t="shared" si="4"/>
+        <v>5200</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="5"/>
+        <v>06900</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="7"/>
+        <v>13500</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="0"/>
         <v>5200</v>
       </c>
-      <c r="I5" t="str">
+      <c r="M5">
         <f t="shared" si="1"/>
-        <v>06900</v>
-      </c>
-      <c r="J5" t="str">
+        <v>6900</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="K5" t="str">
+      <c r="O5">
         <f t="shared" si="3"/>
-        <v>13500</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="4"/>
-        <v>5200</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="5"/>
-        <v>6900</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="7"/>
         <v>13500</v>
       </c>
       <c r="Q5" t="str">
@@ -910,7 +922,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;China/Taiwan on 144.6400MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;69,52,0 135,52,0 135,20,0 69,20,0 69,52,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -934,35 +946,35 @@
         <v>144.5750</v>
       </c>
       <c r="H6" t="str">
+        <f t="shared" si="4"/>
+        <v>-3200</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="5"/>
+        <v>16500</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v>-4900</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="7"/>
+        <v>18000</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="0"/>
         <v>-3200</v>
       </c>
-      <c r="I6" t="str">
+      <c r="M6">
         <f t="shared" si="1"/>
         <v>16500</v>
       </c>
-      <c r="J6" t="str">
+      <c r="N6">
         <f t="shared" si="2"/>
         <v>-4900</v>
       </c>
-      <c r="K6" t="str">
+      <c r="O6">
         <f t="shared" si="3"/>
-        <v>18000</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
-        <v>-3200</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="5"/>
-        <v>16500</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="6"/>
-        <v>-4900</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="7"/>
         <v>18000</v>
       </c>
       <c r="Q6" t="str">
@@ -974,7 +986,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;New Zealand on 144.5750MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;165,-32,0 180,-32,0 180,-49,0 165,-49,0 165,-32,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -998,35 +1010,35 @@
         <v>145.1750</v>
       </c>
       <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>-0900</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="5"/>
+        <v>11100</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>-4500</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="7"/>
+        <v>15400</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="0"/>
-        <v>-0900</v>
-      </c>
-      <c r="I7" t="str">
+        <v>-900</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="1"/>
         <v>11100</v>
       </c>
-      <c r="J7" t="str">
+      <c r="N7">
         <f t="shared" si="2"/>
         <v>-4500</v>
       </c>
-      <c r="K7" t="str">
+      <c r="O7">
         <f t="shared" si="3"/>
-        <v>15400</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
-        <v>-900</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="5"/>
-        <v>11100</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="6"/>
-        <v>-4500</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="7"/>
         <v>15400</v>
       </c>
       <c r="Q7" t="str">
@@ -1038,7 +1050,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Austrailia on 145.1750MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;111,-9,0 154,-9,0 154,-45,0 111,-45,0 111,-9,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1062,35 +1074,35 @@
         <v>144.8000</v>
       </c>
       <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>7300</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="5"/>
+        <v>-01200</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v>3600</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="7"/>
+        <v>05000</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="0"/>
         <v>7300</v>
       </c>
-      <c r="I8" t="str">
+      <c r="M8">
         <f t="shared" si="1"/>
-        <v>-01200</v>
-      </c>
-      <c r="J8" t="str">
+        <v>-1200</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="2"/>
         <v>3600</v>
       </c>
-      <c r="K8" t="str">
+      <c r="O8">
         <f t="shared" si="3"/>
-        <v>05000</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
-        <v>7300</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="5"/>
-        <v>-1200</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="6"/>
-        <v>3600</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="7"/>
         <v>5000</v>
       </c>
       <c r="Q8" t="str">
@@ -1102,7 +1114,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Europe on 144.8000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-12,73,0 50,73,0 50,36,0 -12,36,0 -12,73,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1126,35 +1138,35 @@
         <v>144.8000</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" ref="H9:H10" si="10">TEXT(INT(B9),"00") &amp; TEXT((B9-INT(B9))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>3600</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9:I10" si="11">TEXT(INT(C9),"000") &amp; TEXT((C9-INT(C9))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>-02100</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9:J10" si="12">TEXT(INT(D9),"00") &amp; TEXT((D9-INT(D9))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>-3600</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" ref="K9:K10" si="13">TEXT(INT(E9),"000") &amp; TEXT((E9-INT(E9))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>05200</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9:L10" si="14">INT(H9)</f>
+        <f t="shared" ref="L9:L10" si="10">INT(H9)</f>
         <v>3600</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M10" si="15">INT(I9)</f>
+        <f t="shared" ref="M9:M10" si="11">INT(I9)</f>
         <v>-2100</v>
       </c>
       <c r="N9">
-        <f t="shared" ref="N9:N10" si="16">INT(J9)</f>
+        <f t="shared" ref="N9:N10" si="12">INT(J9)</f>
         <v>-3600</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O10" si="17">INT(K9)</f>
+        <f t="shared" ref="O9:O10" si="13">INT(K9)</f>
         <v>5200</v>
       </c>
       <c r="Q9" t="str">
@@ -1166,7 +1178,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Africa on 144.8000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-21,36,0 52,36,0 52,-36,0 -21,-36,0 -21,36,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1190,35 +1202,35 @@
         <v>144.8000</v>
       </c>
       <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v>7500</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="5"/>
+        <v>05000</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v>5200</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="7"/>
+        <v>18000</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="10"/>
         <v>7500</v>
       </c>
-      <c r="I10" t="str">
+      <c r="M10">
         <f t="shared" si="11"/>
-        <v>05000</v>
-      </c>
-      <c r="J10" t="str">
+        <v>5000</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="12"/>
         <v>5200</v>
       </c>
-      <c r="K10" t="str">
+      <c r="O10">
         <f t="shared" si="13"/>
-        <v>18000</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="14"/>
-        <v>7500</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="15"/>
-        <v>5000</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="16"/>
-        <v>5200</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="17"/>
         <v>18000</v>
       </c>
       <c r="Q10" t="str">
@@ -1230,7 +1242,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Russia on 144.8000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;50,75,0 180,75,0 180,52,0 50,52,0 50,75,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1254,35 +1266,35 @@
         <v>144.3900</v>
       </c>
       <c r="H11" t="str">
-        <f>TEXT(INT(B11),"00") &amp; TEXT((B11-INT(B11))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>8000</v>
       </c>
       <c r="I11" t="str">
-        <f>TEXT(INT(C11),"000") &amp; TEXT((C11-INT(C11))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>-16900</v>
       </c>
       <c r="J11" t="str">
-        <f>TEXT(INT(D11),"00") &amp; TEXT((D11-INT(D11))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>5000</v>
       </c>
       <c r="K11" t="str">
-        <f>TEXT(INT(E11),"000") &amp; TEXT((E11-INT(E11))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>-13000</v>
       </c>
       <c r="L11">
-        <f>INT(H11)</f>
+        <f t="shared" ref="L11:O16" si="14">INT(H11)</f>
         <v>8000</v>
       </c>
       <c r="M11">
-        <f>INT(I11)</f>
+        <f t="shared" si="14"/>
         <v>-16900</v>
       </c>
       <c r="N11">
-        <f>INT(J11)</f>
+        <f t="shared" si="14"/>
         <v>5000</v>
       </c>
       <c r="O11">
-        <f>INT(K11)</f>
+        <f t="shared" si="14"/>
         <v>-13000</v>
       </c>
       <c r="Q11" t="str">
@@ -1294,7 +1306,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Alaska on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-169,80,0 -130,80,0 -130,50,0 -169,50,0 -169,80,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1318,35 +1330,35 @@
         <v>144.3900</v>
       </c>
       <c r="H12" t="str">
-        <f>TEXT(INT(B12),"00") &amp; TEXT((B12-INT(B12))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>2600</v>
       </c>
       <c r="I12" t="str">
-        <f>TEXT(INT(C12),"000") &amp; TEXT((C12-INT(C12))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>-16500</v>
       </c>
       <c r="J12" t="str">
-        <f>TEXT(INT(D12),"00") &amp; TEXT((D12-INT(D12))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
       <c r="K12" t="str">
-        <f>TEXT(INT(E12),"000") &amp; TEXT((E12-INT(E12))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>-15300</v>
       </c>
       <c r="L12">
-        <f>INT(H12)</f>
+        <f t="shared" si="14"/>
         <v>2600</v>
       </c>
       <c r="M12">
-        <f>INT(I12)</f>
+        <f t="shared" si="14"/>
         <v>-16500</v>
       </c>
       <c r="N12">
-        <f>INT(J12)</f>
+        <f t="shared" si="14"/>
         <v>1500</v>
       </c>
       <c r="O12">
-        <f>INT(K12)</f>
+        <f t="shared" si="14"/>
         <v>-15300</v>
       </c>
       <c r="Q12" t="str">
@@ -1358,7 +1370,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Hawaii on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-165,26,0 -153,26,0 -153,15,0 -165,15,0 -165,26,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1382,35 +1394,35 @@
         <v>145.5700</v>
       </c>
       <c r="H13" t="str">
-        <f>TEXT(INT(B13),"00") &amp; TEXT((B13-INT(B13))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>0300</v>
       </c>
       <c r="I13" t="str">
-        <f>TEXT(INT(C13),"000") &amp; TEXT((C13-INT(C13))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>-07000</v>
       </c>
       <c r="J13" t="str">
-        <f>TEXT(INT(D13),"00") &amp; TEXT((D13-INT(D13))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>-3000</v>
       </c>
       <c r="K13" t="str">
-        <f>TEXT(INT(E13),"000") &amp; TEXT((E13-INT(E13))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>-03300</v>
       </c>
       <c r="L13">
-        <f>INT(H13)</f>
+        <f t="shared" si="14"/>
         <v>300</v>
       </c>
       <c r="M13">
-        <f>INT(I13)</f>
+        <f t="shared" si="14"/>
         <v>-7000</v>
       </c>
       <c r="N13">
-        <f>INT(J13)</f>
+        <f t="shared" si="14"/>
         <v>-3000</v>
       </c>
       <c r="O13">
-        <f>INT(K13)</f>
+        <f t="shared" si="14"/>
         <v>-3300</v>
       </c>
       <c r="Q13" t="str">
@@ -1422,7 +1434,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Brazil on 145.5700MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-70,3,0 -33,3,0 -33,-30,0 -70,-30,0 -70,3,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1446,35 +1458,35 @@
         <v>144.6600</v>
       </c>
       <c r="H14" t="str">
-        <f>TEXT(INT(B14),"00") &amp; TEXT((B14-INT(B14))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>4500</v>
       </c>
       <c r="I14" t="str">
-        <f>TEXT(INT(C14),"000") &amp; TEXT((C14-INT(C14))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>12900</v>
       </c>
       <c r="J14" t="str">
-        <f>TEXT(INT(D14),"00") &amp; TEXT((D14-INT(D14))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>3000</v>
       </c>
       <c r="K14" t="str">
-        <f>TEXT(INT(E14),"000") &amp; TEXT((E14-INT(E14))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>14600</v>
       </c>
       <c r="L14">
-        <f>INT(H14)</f>
+        <f t="shared" si="14"/>
         <v>4500</v>
       </c>
       <c r="M14">
-        <f>INT(I14)</f>
+        <f t="shared" si="14"/>
         <v>12900</v>
       </c>
       <c r="N14">
-        <f>INT(J14)</f>
+        <f t="shared" si="14"/>
         <v>3000</v>
       </c>
       <c r="O14">
-        <f>INT(K14)</f>
+        <f t="shared" si="14"/>
         <v>14600</v>
       </c>
       <c r="Q14" t="str">
@@ -1486,7 +1498,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Japan on 144.6600MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;129,45,0 146,45,0 146,30,0 129,30,0 129,45,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1510,35 +1522,35 @@
         <v>145.5300</v>
       </c>
       <c r="H15" t="str">
-        <f>TEXT(INT(B15),"00") &amp; TEXT((B15-INT(B15))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>2036</v>
       </c>
       <c r="I15" t="str">
-        <f>TEXT(INT(C15),"000") &amp; TEXT((C15-INT(C15))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>09700</v>
       </c>
       <c r="J15" t="str">
-        <f>TEXT(INT(D15),"00") &amp; TEXT((D15-INT(D15))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>0500</v>
       </c>
       <c r="K15" t="str">
-        <f>TEXT(INT(E15),"000") &amp; TEXT((E15-INT(E15))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>10600</v>
       </c>
       <c r="L15">
-        <f>INT(H15)</f>
+        <f t="shared" si="14"/>
         <v>2036</v>
       </c>
       <c r="M15">
-        <f>INT(I15)</f>
+        <f t="shared" si="14"/>
         <v>9700</v>
       </c>
       <c r="N15">
-        <f>INT(J15)</f>
+        <f t="shared" si="14"/>
         <v>500</v>
       </c>
       <c r="O15">
-        <f>INT(K15)</f>
+        <f t="shared" si="14"/>
         <v>10600</v>
       </c>
       <c r="Q15" t="str">
@@ -1550,7 +1562,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Thailand on 145.5300MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;97,20.6,0 106,20.6,0 106,5,0 97,5,0 97,20.6,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1574,47 +1586,47 @@
         <v>144.5250</v>
       </c>
       <c r="H16" t="str">
-        <f>TEXT(INT(B16),"00") &amp; TEXT((B16-INT(B16))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>2230</v>
       </c>
       <c r="I16" t="str">
-        <f>TEXT(INT(C16),"000") &amp; TEXT((C16-INT(C16))*60,"00")</f>
-        <v>11348</v>
+        <f t="shared" si="5"/>
+        <v>11347</v>
       </c>
       <c r="J16" t="str">
-        <f>TEXT(INT(D16),"00") &amp; TEXT((D16-INT(D16))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>2200</v>
       </c>
       <c r="K16" t="str">
-        <f>TEXT(INT(E16),"000") &amp; TEXT((E16-INT(E16))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>11430</v>
       </c>
       <c r="L16">
-        <f>INT(H16)</f>
+        <f t="shared" si="14"/>
         <v>2230</v>
       </c>
       <c r="M16">
-        <f>INT(I16)</f>
-        <v>11348</v>
+        <f t="shared" si="14"/>
+        <v>11347</v>
       </c>
       <c r="N16">
-        <f>INT(J16)</f>
+        <f t="shared" si="14"/>
         <v>2200</v>
       </c>
       <c r="O16">
-        <f>INT(K16)</f>
+        <f t="shared" si="14"/>
         <v>11430</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="8"/>
-        <v>if (iLat &gt;= 2200 &amp;&amp; iLat &lt;= 2230 &amp;&amp; iLon &gt;= 11348 &amp;&amp; iLon &lt;= 11430) freqSelected = 2;    //Hong Kong on 144.5250MHz</v>
+        <v>if (iLat &gt;= 2200 &amp;&amp; iLat &lt;= 2230 &amp;&amp; iLon &gt;= 11347 &amp;&amp; iLon &lt;= 11430) freqSelected = 2;    //Hong Kong on 144.5250MHz</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="9"/>
         <v>&lt;Placemark&gt;&lt;name&gt;Hong Kong on 144.5250MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;113.8,22.5,0 114.5,22.5,0 114.5,22,0 113.8,22,0 113.8,22.5,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1638,19 +1650,19 @@
         <v>000.0000</v>
       </c>
       <c r="H17" t="str">
-        <f>TEXT(INT(B17),"00") &amp; TEXT((B17-INT(B17))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>6100</v>
       </c>
       <c r="I17" t="str">
-        <f>TEXT(INT(C17),"000") &amp; TEXT((C17-INT(C17))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>-00800</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ref="I17:K17" si="18">TEXT(INT(D17),"00") &amp; TEXT((D17-INT(D17))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>4900</v>
       </c>
       <c r="K17" t="str">
-        <f>TEXT(INT(E17),"000") &amp; TEXT((E17-INT(E17))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>00200</v>
       </c>
       <c r="L17">
@@ -1658,15 +1670,15 @@
         <v>6100</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17:O17" si="19">INT(I17)</f>
+        <f t="shared" ref="M17:O17" si="15">INT(I17)</f>
         <v>-800</v>
       </c>
       <c r="N17">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>4900</v>
       </c>
       <c r="O17">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>200</v>
       </c>
       <c r="Q17" t="str">
@@ -1678,7 +1690,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;UK on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-8,61,0 2,61,0 2,49,0 -8,49,0 -8,61,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1702,19 +1714,19 @@
         <v>000.0000</v>
       </c>
       <c r="H18" t="str">
-        <f>TEXT(INT(B18),"00") &amp; TEXT((B18-INT(B18))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>1912</v>
       </c>
       <c r="I18" t="str">
-        <f>TEXT(INT(C18),"000") &amp; TEXT((C18-INT(C18))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>04200</v>
       </c>
       <c r="J18" t="str">
-        <f>TEXT(INT(D18),"00") &amp; TEXT((D18-INT(D18))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>1148</v>
       </c>
       <c r="K18" t="str">
-        <f>TEXT(INT(E18),"000") &amp; TEXT((E18-INT(E18))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>05442</v>
       </c>
       <c r="L18">
@@ -1722,15 +1734,15 @@
         <v>1912</v>
       </c>
       <c r="M18">
-        <f>INT(I18)</f>
+        <f t="shared" ref="M18:O19" si="16">INT(I18)</f>
         <v>4200</v>
       </c>
       <c r="N18">
-        <f>INT(J18)</f>
+        <f t="shared" si="16"/>
         <v>1148</v>
       </c>
       <c r="O18">
-        <f>INT(K18)</f>
+        <f t="shared" si="16"/>
         <v>5442</v>
       </c>
       <c r="Q18" t="str">
@@ -1742,7 +1754,7 @@
         <v>&lt;Placemark&gt;&lt;name&gt;Yemen on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;42,19.2,0 54.7,19.2,0 54.7,11.8,0 42,11.8,0 42,19.2,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1766,19 +1778,19 @@
         <v>000.0000</v>
       </c>
       <c r="H19" t="str">
-        <f>TEXT(INT(B19),"00") &amp; TEXT((B19-INT(B19))*60,"00")</f>
+        <f t="shared" si="4"/>
         <v>4306</v>
       </c>
       <c r="I19" t="str">
-        <f>TEXT(INT(C19),"000") &amp; TEXT((C19-INT(C19))*60,"00")</f>
+        <f t="shared" si="5"/>
         <v>13100</v>
       </c>
       <c r="J19" t="str">
-        <f>TEXT(INT(D19),"00") &amp; TEXT((D19-INT(D19))*60,"00")</f>
+        <f t="shared" si="6"/>
         <v>3742</v>
       </c>
       <c r="K19" t="str">
-        <f>TEXT(INT(E19),"000") &amp; TEXT((E19-INT(E19))*60,"00")</f>
+        <f t="shared" si="7"/>
         <v>12400</v>
       </c>
       <c r="L19">
@@ -1786,15 +1798,15 @@
         <v>4306</v>
       </c>
       <c r="M19">
-        <f>INT(I19)</f>
+        <f t="shared" si="16"/>
         <v>13100</v>
       </c>
       <c r="N19">
-        <f>INT(J19)</f>
+        <f t="shared" si="16"/>
         <v>3742</v>
       </c>
       <c r="O19">
-        <f>INT(K19)</f>
+        <f t="shared" si="16"/>
         <v>12400</v>
       </c>
       <c r="Q19" t="str">
@@ -1806,8 +1818,264 @@
         <v>&lt;Placemark&gt;&lt;name&gt;North Korea on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;131,43.1,0 124,43.1,0 124,37.7,0 131,37.7,0 131,43.1,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S25" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>38.11</v>
+      </c>
+      <c r="C22">
+        <v>-97.95</v>
+      </c>
+      <c r="D22">
+        <v>38.07</v>
+      </c>
+      <c r="E22">
+        <v>-97.89</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP(F22, Freq[], 2, TRUE)</f>
+        <v>144.5250</v>
+      </c>
+      <c r="H22" t="str">
+        <f>IF(B22&gt;=0,"","-") &amp; TEXT(INT(ABS(B22)),"00") &amp; TEXT(INT((ABS(B22)-INT(ABS(B22)))*60),"00")</f>
+        <v>3806</v>
+      </c>
+      <c r="I22" t="str">
+        <f>IF(C22&gt;=0,"","-") &amp; TEXT(INT(ABS(C22)),"000") &amp; TEXT(INT((ABS(C22)-INT(ABS(C22)))*60),"00")</f>
+        <v>-09757</v>
+      </c>
+      <c r="J22" t="str">
+        <f>IF(D22&gt;=0,"","-") &amp; TEXT(INT(ABS(D22)),"00") &amp; TEXT(INT((ABS(D22)-INT(ABS(D22)))*60),"00")</f>
+        <v>3804</v>
+      </c>
+      <c r="K22" t="str">
+        <f>IF(E22&gt;=0,"","-") &amp; TEXT(INT(ABS(E22)),"000") &amp; TEXT(INT((ABS(E22)-INT(ABS(E22)))*60),"00")</f>
+        <v>-09753</v>
+      </c>
+      <c r="L22">
+        <f>INT(H22)</f>
+        <v>3806</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ref="M22" si="17">INT(I22)</f>
+        <v>-9757</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22" si="18">INT(J22)</f>
+        <v>3804</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ref="O22" si="19">INT(K22)</f>
+        <v>-9753</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" ref="Q22" si="20">_xlfn.CONCAT("if (iLat &gt;= ", N22, " &amp;&amp; iLat &lt;= ", L22, " &amp;&amp; iLon &gt;= ", M22, " &amp;&amp; iLon &lt;= ", O22, ") freqSelected = ", F22, ";    //", A22, " on ", G22, "MHz")</f>
+        <v>if (iLat &gt;= 3804 &amp;&amp; iLat &lt;= 3806 &amp;&amp; iLon &gt;= -9757 &amp;&amp; iLon &lt;= -9753) freqSelected = 2;    //Home on 144.5250MHz</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" ref="S22" si="21">_xlfn.CONCAT("&lt;Placemark&gt;&lt;name&gt;",A22, " on ", G22, "MHz","&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;",C22, ",", B22, ",0 ",E22, ",", B22, ",0 ",E22, ",", D22, ",0 ",C22, ",", D22, ",0 ",C22, ",", B22, ",0 ","&lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;")</f>
+        <v>&lt;Placemark&gt;&lt;name&gt;Home on 144.5250MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-97.95,38.11,0 -97.89,38.11,0 -97.89,38.07,0 -97.95,38.07,0 -97.95,38.11,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23">
+        <v>38.03</v>
+      </c>
+      <c r="C23">
+        <v>-97.96</v>
+      </c>
+      <c r="D23">
+        <v>38.01</v>
+      </c>
+      <c r="E23">
+        <v>-97.88</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP(F23, Freq[], 2, TRUE)</f>
+        <v>000.0000</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" ref="H23:H25" si="22">IF(B23&gt;=0,"","-") &amp; TEXT(INT(ABS(B23)),"00") &amp; TEXT(INT((ABS(B23)-INT(ABS(B23)))*60),"00")</f>
+        <v>3801</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" ref="I23:I25" si="23">IF(C23&gt;=0,"","-") &amp; TEXT(INT(ABS(C23)),"000") &amp; TEXT(INT((ABS(C23)-INT(ABS(C23)))*60),"00")</f>
+        <v>-09757</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" ref="J23:J25" si="24">IF(D23&gt;=0,"","-") &amp; TEXT(INT(ABS(D23)),"00") &amp; TEXT(INT((ABS(D23)-INT(ABS(D23)))*60),"00")</f>
+        <v>3800</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" ref="K23:K25" si="25">IF(E23&gt;=0,"","-") &amp; TEXT(INT(ABS(E23)),"000") &amp; TEXT(INT((ABS(E23)-INT(ABS(E23)))*60),"00")</f>
+        <v>-09752</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:L24" si="26">INT(H23)</f>
+        <v>3801</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:M24" si="27">INT(I23)</f>
+        <v>-9757</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:N24" si="28">INT(J23)</f>
+        <v>3800</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23:O24" si="29">INT(K23)</f>
+        <v>-9752</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" ref="Q23:Q24" si="30">_xlfn.CONCAT("if (iLat &gt;= ", N23, " &amp;&amp; iLat &lt;= ", L23, " &amp;&amp; iLon &gt;= ", M23, " &amp;&amp; iLon &lt;= ", O23, ") freqSelected = ", F23, ";    //", A23, " on ", G23, "MHz")</f>
+        <v>if (iLat &gt;= 3800 &amp;&amp; iLat &lt;= 3801 &amp;&amp; iLon &gt;= -9757 &amp;&amp; iLon &lt;= -9752) freqSelected = 0;    //South Hutch on 000.0000MHz</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" ref="S23:S24" si="31">_xlfn.CONCAT("&lt;Placemark&gt;&lt;name&gt;",A23, " on ", G23, "MHz","&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;",C23, ",", B23, ",0 ",E23, ",", B23, ",0 ",E23, ",", D23, ",0 ",C23, ",", D23, ",0 ",C23, ",", B23, ",0 ","&lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;")</f>
+        <v>&lt;Placemark&gt;&lt;name&gt;South Hutch on 000.0000MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-97.96,38.03,0 -97.88,38.03,0 -97.88,38.01,0 -97.96,38.01,0 -97.96,38.03,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <v>38.06</v>
+      </c>
+      <c r="C24">
+        <v>-97.72</v>
+      </c>
+      <c r="D24">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>-97.62</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP(F24, Freq[], 2, TRUE)</f>
+        <v>144.3900</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="22"/>
+        <v>3803</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="23"/>
+        <v>-09743</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="24"/>
+        <v>3800</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="25"/>
+        <v>-09737</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="26"/>
+        <v>3803</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="27"/>
+        <v>-9743</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="28"/>
+        <v>3800</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="29"/>
+        <v>-9737</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="30"/>
+        <v>if (iLat &gt;= 3800 &amp;&amp; iLat &lt;= 3803 &amp;&amp; iLon &gt;= -9743 &amp;&amp; iLon &lt;= -9737) freqSelected = 1;    //Burrton on 144.3900MHz</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="31"/>
+        <v>&lt;Placemark&gt;&lt;name&gt;Burrton on 144.3900MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-97.72,38.06,0 -97.62,38.06,0 -97.62,38,0 -97.72,38,0 -97.72,38.06,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>38.04</v>
+      </c>
+      <c r="C25">
+        <v>-97.84</v>
+      </c>
+      <c r="D25">
+        <v>38.01</v>
+      </c>
+      <c r="E25">
+        <v>-97.74</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP(F25, Freq[], 2, TRUE)</f>
+        <v>144.5750</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="22"/>
+        <v>3802</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="23"/>
+        <v>-09750</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="24"/>
+        <v>3800</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="25"/>
+        <v>-09744</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25" si="32">INT(H25)</f>
+        <v>3802</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25" si="33">INT(I25)</f>
+        <v>-9750</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25" si="34">INT(J25)</f>
+        <v>3800</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ref="O25" si="35">INT(K25)</f>
+        <v>-9744</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" ref="Q25" si="36">_xlfn.CONCAT("if (iLat &gt;= ", N25, " &amp;&amp; iLat &lt;= ", L25, " &amp;&amp; iLon &gt;= ", M25, " &amp;&amp; iLon &lt;= ", O25, ") freqSelected = ", F25, ";    //", A25, " on ", G25, "MHz")</f>
+        <v>if (iLat &gt;= 3800 &amp;&amp; iLat &lt;= 3802 &amp;&amp; iLon &gt;= -9750 &amp;&amp; iLon &lt;= -9744) freqSelected = 3;    //US50 on 144.5750MHz</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" ref="S25" si="37">_xlfn.CONCAT("&lt;Placemark&gt;&lt;name&gt;",A25, " on ", G25, "MHz","&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;",C25, ",", B25, ",0 ",E25, ",", B25, ",0 ",E25, ",", D25, ",0 ",C25, ",", D25, ",0 ",C25, ",", B25, ",0 ","&lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;")</f>
+        <v>&lt;Placemark&gt;&lt;name&gt;US50 on 144.5750MHz&lt;/name&gt;&lt;styleUrl&gt;#poly-000000-1200-77-nodesc&lt;/styleUrl&gt;&lt;Polygon&gt;&lt;outerBoundaryIs&gt;&lt;LinearRing&gt;&lt;tessellate&gt;1&lt;/tessellate&gt;&lt;coordinates&gt;-97.84,38.04,0 -97.74,38.04,0 -97.74,38.01,0 -97.84,38.01,0 -97.84,38.04,0 &lt;/coordinates&gt;&lt;/LinearRing&gt;&lt;/outerBoundaryIs&gt;&lt;/Polygon&gt;&lt;/Placemark&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S31" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1825,13 +2093,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1842,7 +2110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1853,7 +2121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1864,7 +2132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1875,7 +2143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1886,7 +2154,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1897,7 +2165,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1908,7 +2176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1919,7 +2187,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1930,7 +2198,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1941,7 +2209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1952,7 +2220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>99</v>
       </c>

</xml_diff>